<commit_message>
r24 && r26 e0/3 int change ipv4
</commit_message>
<xml_diff>
--- a/lab07/1.xlsx
+++ b/lab07/1.xlsx
@@ -908,9 +908,6 @@
     <t>2001:ABCD:0070:2324::23/64</t>
   </si>
   <si>
-    <t>100.10.10.202/27</t>
-  </si>
-  <si>
     <t>2001:ABCD:0060:2124::24/64</t>
   </si>
   <si>
@@ -938,9 +935,6 @@
     <t>2001:ABCD:0030:2528::25/64</t>
   </si>
   <si>
-    <t>100.10.10.205/27</t>
-  </si>
-  <si>
     <t>2001:ABCD:0030:2628::26/64</t>
   </si>
   <si>
@@ -993,6 +987,12 @@
   </si>
   <si>
     <t>2001:ABCD:0010:1520::20/64</t>
+  </si>
+  <si>
+    <t>200.20.20.24/27</t>
+  </si>
+  <si>
+    <t>200.20.20.26/27</t>
   </si>
 </sst>
 </file>
@@ -1852,7 +1852,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -2044,7 +2044,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2065,21 +2122,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2104,49 +2146,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3858,8 +3861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3874,19 +3877,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="68" t="s">
         <v>274</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="76"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="70"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="68" t="s">
         <v>129</v>
       </c>
-      <c r="B2" s="76"/>
+      <c r="B2" s="70"/>
       <c r="C2" s="41" t="s">
         <v>0</v>
       </c>
@@ -3898,7 +3901,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="94" t="s">
+      <c r="A3" s="74" t="s">
         <v>131</v>
       </c>
       <c r="B3" s="42" t="s">
@@ -3915,7 +3918,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="89"/>
+      <c r="A4" s="65"/>
       <c r="B4" s="9" t="s">
         <v>137</v>
       </c>
@@ -3928,14 +3931,14 @@
       <c r="E4" s="26" t="s">
         <v>182</v>
       </c>
-      <c r="I4" s="66" t="s">
-        <v>311</v>
-      </c>
-      <c r="J4" s="67"/>
-      <c r="K4" s="67"/>
+      <c r="I4" s="85" t="s">
+        <v>309</v>
+      </c>
+      <c r="J4" s="86"/>
+      <c r="K4" s="86"/>
     </row>
     <row r="5" spans="1:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="89"/>
+      <c r="A5" s="65"/>
       <c r="B5" s="9" t="s">
         <v>133</v>
       </c>
@@ -3948,12 +3951,12 @@
       <c r="E5" s="26" t="s">
         <v>182</v>
       </c>
-      <c r="I5" s="67"/>
-      <c r="J5" s="67"/>
-      <c r="K5" s="67"/>
+      <c r="I5" s="86"/>
+      <c r="J5" s="86"/>
+      <c r="K5" s="86"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="95"/>
+      <c r="A6" s="75"/>
       <c r="B6" s="11" t="s">
         <v>134</v>
       </c>
@@ -3966,12 +3969,12 @@
       <c r="E6" s="35" t="s">
         <v>182</v>
       </c>
-      <c r="I6" s="67"/>
-      <c r="J6" s="67"/>
-      <c r="K6" s="67"/>
+      <c r="I6" s="86"/>
+      <c r="J6" s="86"/>
+      <c r="K6" s="86"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="89" t="s">
+      <c r="A7" s="65" t="s">
         <v>135</v>
       </c>
       <c r="B7" s="7" t="s">
@@ -3988,7 +3991,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="89"/>
+      <c r="A8" s="65"/>
       <c r="B8" s="25" t="s">
         <v>137</v>
       </c>
@@ -4003,7 +4006,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="89"/>
+      <c r="A9" s="65"/>
       <c r="B9" s="9" t="s">
         <v>133</v>
       </c>
@@ -4018,7 +4021,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="95"/>
+      <c r="A10" s="75"/>
       <c r="B10" s="11" t="s">
         <v>134</v>
       </c>
@@ -4033,7 +4036,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="92" t="s">
+      <c r="A11" s="71" t="s">
         <v>136</v>
       </c>
       <c r="B11" s="7" t="s">
@@ -4048,16 +4051,16 @@
       <c r="E11" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="H11" s="77" t="s">
+      <c r="H11" s="91" t="s">
         <v>272</v>
       </c>
-      <c r="I11" s="78"/>
-      <c r="J11" s="78"/>
-      <c r="K11" s="78"/>
-      <c r="L11" s="79"/>
+      <c r="I11" s="92"/>
+      <c r="J11" s="92"/>
+      <c r="K11" s="92"/>
+      <c r="L11" s="93"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="93"/>
+      <c r="A12" s="72"/>
       <c r="B12" s="9" t="s">
         <v>137</v>
       </c>
@@ -4070,7 +4073,7 @@
       <c r="E12" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="H12" s="80" t="s">
+      <c r="H12" s="94" t="s">
         <v>269</v>
       </c>
       <c r="I12" s="49" t="s">
@@ -4087,7 +4090,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="93"/>
+      <c r="A13" s="72"/>
       <c r="B13" s="9" t="s">
         <v>133</v>
       </c>
@@ -4100,7 +4103,7 @@
       <c r="E13" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="H13" s="81"/>
+      <c r="H13" s="95"/>
       <c r="I13" s="45" t="s">
         <v>137</v>
       </c>
@@ -4115,20 +4118,20 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="93"/>
-      <c r="B14" s="72" t="s">
+      <c r="A14" s="72"/>
+      <c r="B14" s="83" t="s">
         <v>134</v>
       </c>
-      <c r="C14" s="70" t="s">
+      <c r="C14" s="89" t="s">
         <v>169</v>
       </c>
-      <c r="D14" s="68" t="s">
+      <c r="D14" s="87" t="s">
         <v>165</v>
       </c>
-      <c r="E14" s="72" t="s">
+      <c r="E14" s="83" t="s">
         <v>184</v>
       </c>
-      <c r="H14" s="82"/>
+      <c r="H14" s="96"/>
       <c r="I14" s="51" t="s">
         <v>133</v>
       </c>
@@ -4145,12 +4148,12 @@
     <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="73"/>
       <c r="B15" s="73"/>
-      <c r="C15" s="71"/>
-      <c r="D15" s="69"/>
+      <c r="C15" s="90"/>
+      <c r="D15" s="88"/>
       <c r="E15" s="73"/>
     </row>
     <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="92" t="s">
+      <c r="A16" s="71" t="s">
         <v>138</v>
       </c>
       <c r="B16" s="7" t="s">
@@ -4165,16 +4168,16 @@
       <c r="E16" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="H16" s="77" t="s">
+      <c r="H16" s="91" t="s">
         <v>273</v>
       </c>
-      <c r="I16" s="78"/>
-      <c r="J16" s="78"/>
-      <c r="K16" s="78"/>
-      <c r="L16" s="79"/>
+      <c r="I16" s="92"/>
+      <c r="J16" s="92"/>
+      <c r="K16" s="92"/>
+      <c r="L16" s="93"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="93"/>
+      <c r="A17" s="72"/>
       <c r="B17" s="9" t="s">
         <v>137</v>
       </c>
@@ -4187,7 +4190,7 @@
       <c r="E17" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="H17" s="83" t="s">
+      <c r="H17" s="97" t="s">
         <v>264</v>
       </c>
       <c r="I17" s="56" t="s">
@@ -4204,7 +4207,7 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="93"/>
+      <c r="A18" s="72"/>
       <c r="B18" s="9" t="s">
         <v>133</v>
       </c>
@@ -4217,7 +4220,7 @@
       <c r="E18" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="H18" s="83"/>
+      <c r="H18" s="97"/>
       <c r="I18" s="45" t="s">
         <v>137</v>
       </c>
@@ -4245,7 +4248,7 @@
       <c r="E19" s="53" t="s">
         <v>185</v>
       </c>
-      <c r="H19" s="84"/>
+      <c r="H19" s="98"/>
       <c r="I19" s="45" t="s">
         <v>133</v>
       </c>
@@ -4270,7 +4273,7 @@
         <v>245</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>246</v>
@@ -4287,18 +4290,18 @@
         <v>247</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="H21" s="74" t="s">
+      <c r="H21" s="68" t="s">
         <v>283</v>
       </c>
-      <c r="I21" s="75"/>
-      <c r="J21" s="75"/>
-      <c r="K21" s="75"/>
-      <c r="L21" s="76"/>
+      <c r="I21" s="69"/>
+      <c r="J21" s="69"/>
+      <c r="K21" s="69"/>
+      <c r="L21" s="70"/>
     </row>
     <row r="22" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="20" t="s">
@@ -4312,7 +4315,7 @@
         <v>257</v>
       </c>
       <c r="E22" s="56"/>
-      <c r="H22" s="85" t="s">
+      <c r="H22" s="82" t="s">
         <v>284</v>
       </c>
       <c r="I22" s="49" t="s">
@@ -4340,12 +4343,12 @@
         <v>254</v>
       </c>
       <c r="E23" s="44"/>
-      <c r="H23" s="86"/>
+      <c r="H23" s="80"/>
       <c r="I23" s="45" t="s">
         <v>137</v>
       </c>
       <c r="J23" s="45" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="K23" s="47" t="s">
         <v>294</v>
@@ -4366,12 +4369,12 @@
         <v>255</v>
       </c>
       <c r="E24" s="44"/>
-      <c r="H24" s="87"/>
+      <c r="H24" s="81"/>
       <c r="I24" s="51" t="s">
         <v>133</v>
       </c>
       <c r="J24" s="45" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="K24" s="47" t="s">
         <v>295</v>
@@ -4392,17 +4395,17 @@
         <v>256</v>
       </c>
       <c r="E25" s="44"/>
-      <c r="H25" s="85" t="s">
+      <c r="H25" s="82" t="s">
         <v>285</v>
       </c>
       <c r="I25" s="49" t="s">
         <v>132</v>
       </c>
       <c r="J25" s="45" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="K25" s="44" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L25" s="50" t="s">
         <v>289</v>
@@ -4420,15 +4423,15 @@
         <v>227</v>
       </c>
       <c r="E26" s="44"/>
-      <c r="H26" s="86"/>
+      <c r="H26" s="80"/>
       <c r="I26" s="58" t="s">
         <v>137</v>
       </c>
       <c r="J26" s="45" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="K26" s="47" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="L26" s="46" t="s">
         <v>289</v>
@@ -4446,79 +4449,79 @@
         <v>228</v>
       </c>
       <c r="E27" s="44"/>
-      <c r="H27" s="86"/>
+      <c r="H27" s="80"/>
       <c r="I27" s="44" t="s">
         <v>133</v>
       </c>
       <c r="J27" s="45" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="K27" s="47" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L27" s="46" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H28" s="87"/>
+      <c r="H28" s="81"/>
       <c r="I28" s="47" t="s">
         <v>134</v>
       </c>
-      <c r="J28" s="45" t="s">
-        <v>296</v>
+      <c r="J28" s="99" t="s">
+        <v>323</v>
       </c>
       <c r="K28" s="47" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L28" s="48" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H29" s="85" t="s">
+      <c r="H29" s="82" t="s">
         <v>286</v>
       </c>
       <c r="I29" s="49" t="s">
         <v>132</v>
       </c>
       <c r="J29" s="45" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="K29" s="47" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="L29" s="50" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="96" t="s">
+      <c r="A30" s="76" t="s">
         <v>275</v>
       </c>
-      <c r="B30" s="97"/>
-      <c r="C30" s="97"/>
-      <c r="D30" s="97"/>
-      <c r="E30" s="98"/>
-      <c r="H30" s="86"/>
+      <c r="B30" s="77"/>
+      <c r="C30" s="77"/>
+      <c r="D30" s="77"/>
+      <c r="E30" s="78"/>
+      <c r="H30" s="80"/>
       <c r="I30" s="58" t="s">
         <v>137</v>
       </c>
       <c r="J30" s="44" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="K30" s="60" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="L30" s="46" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="99" t="s">
+      <c r="A31" s="79" t="s">
         <v>129</v>
       </c>
-      <c r="B31" s="91"/>
+      <c r="B31" s="67"/>
       <c r="C31" s="44" t="s">
         <v>0</v>
       </c>
@@ -4528,22 +4531,22 @@
       <c r="E31" s="46" t="s">
         <v>130</v>
       </c>
-      <c r="H31" s="86"/>
+      <c r="H31" s="80"/>
       <c r="I31" s="44" t="s">
         <v>133</v>
       </c>
       <c r="J31" s="45" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="K31" s="47" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="L31" s="46" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="86" t="s">
+      <c r="A32" s="80" t="s">
         <v>178</v>
       </c>
       <c r="B32" s="44" t="s">
@@ -4558,22 +4561,22 @@
       <c r="E32" s="46" t="s">
         <v>186</v>
       </c>
-      <c r="H32" s="88"/>
+      <c r="H32" s="84"/>
       <c r="I32" s="62" t="s">
         <v>134</v>
       </c>
       <c r="J32" s="62" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="K32" s="62" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="L32" s="63" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="86"/>
+      <c r="A33" s="80"/>
       <c r="B33" s="44" t="s">
         <v>137</v>
       </c>
@@ -4586,24 +4589,24 @@
       <c r="E33" s="46" t="s">
         <v>186</v>
       </c>
-      <c r="H33" s="85" t="s">
+      <c r="H33" s="82" t="s">
         <v>287</v>
       </c>
       <c r="I33" s="49" t="s">
         <v>132</v>
       </c>
       <c r="J33" s="64" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="K33" s="43" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="L33" s="50" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="86"/>
+      <c r="A34" s="80"/>
       <c r="B34" s="45" t="s">
         <v>133</v>
       </c>
@@ -4616,22 +4619,22 @@
       <c r="E34" s="46" t="s">
         <v>186</v>
       </c>
-      <c r="H34" s="86"/>
+      <c r="H34" s="80"/>
       <c r="I34" s="58" t="s">
         <v>137</v>
       </c>
       <c r="J34" s="44" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="K34" s="44" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="L34" s="46" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="87"/>
+      <c r="A35" s="81"/>
       <c r="B35" s="47" t="s">
         <v>134</v>
       </c>
@@ -4644,22 +4647,22 @@
       <c r="E35" s="48" t="s">
         <v>186</v>
       </c>
-      <c r="H35" s="86"/>
+      <c r="H35" s="80"/>
       <c r="I35" s="44" t="s">
         <v>133</v>
       </c>
       <c r="J35" s="45" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="K35" s="62" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="L35" s="46" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="85" t="s">
+      <c r="A36" s="82" t="s">
         <v>179</v>
       </c>
       <c r="B36" s="49" t="s">
@@ -4674,22 +4677,22 @@
       <c r="E36" s="50" t="s">
         <v>187</v>
       </c>
-      <c r="H36" s="87"/>
+      <c r="H36" s="81"/>
       <c r="I36" s="47" t="s">
         <v>134</v>
       </c>
-      <c r="J36" s="65" t="s">
-        <v>306</v>
+      <c r="J36" s="100" t="s">
+        <v>324</v>
       </c>
       <c r="K36" s="47" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="L36" s="61" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="86"/>
+      <c r="A37" s="80"/>
       <c r="B37" s="44" t="s">
         <v>137</v>
       </c>
@@ -4704,7 +4707,7 @@
       </c>
     </row>
     <row r="38" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="87"/>
+      <c r="A38" s="81"/>
       <c r="B38" s="47" t="s">
         <v>133</v>
       </c>
@@ -4719,7 +4722,7 @@
       </c>
     </row>
     <row r="39" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="92" t="s">
+      <c r="A39" s="71" t="s">
         <v>180</v>
       </c>
       <c r="B39" s="16" t="s">
@@ -4736,7 +4739,7 @@
       </c>
     </row>
     <row r="40" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="93"/>
+      <c r="A40" s="72"/>
       <c r="B40" s="17" t="s">
         <v>137</v>
       </c>
@@ -4751,7 +4754,7 @@
       </c>
     </row>
     <row r="41" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="93"/>
+      <c r="A41" s="72"/>
       <c r="B41" s="17" t="s">
         <v>133</v>
       </c>
@@ -4850,13 +4853,13 @@
       <c r="E47" s="44"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="89" t="s">
+      <c r="A50" s="65" t="s">
         <v>276</v>
       </c>
-      <c r="B50" s="90"/>
-      <c r="C50" s="90"/>
-      <c r="D50" s="90"/>
-      <c r="E50" s="91"/>
+      <c r="B50" s="66"/>
+      <c r="C50" s="66"/>
+      <c r="D50" s="66"/>
+      <c r="E50" s="67"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="44" t="s">
@@ -4952,13 +4955,13 @@
       <c r="E57" s="52"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="89" t="s">
+      <c r="A58" s="65" t="s">
         <v>278</v>
       </c>
-      <c r="B58" s="90"/>
-      <c r="C58" s="90"/>
-      <c r="D58" s="90"/>
-      <c r="E58" s="91"/>
+      <c r="B58" s="66"/>
+      <c r="C58" s="66"/>
+      <c r="D58" s="66"/>
+      <c r="E58" s="67"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="44" t="s">
@@ -4979,6 +4982,20 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="I4:K6"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="H21:L21"/>
+    <mergeCell ref="H11:L11"/>
+    <mergeCell ref="H12:H14"/>
+    <mergeCell ref="H16:L16"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="H33:H36"/>
+    <mergeCell ref="H22:H24"/>
+    <mergeCell ref="H25:H28"/>
+    <mergeCell ref="H29:H32"/>
+    <mergeCell ref="A50:E50"/>
     <mergeCell ref="A58:E58"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:B2"/>
@@ -4992,20 +5009,6 @@
     <mergeCell ref="A36:A38"/>
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="A16:A19"/>
-    <mergeCell ref="H33:H36"/>
-    <mergeCell ref="H22:H24"/>
-    <mergeCell ref="H25:H28"/>
-    <mergeCell ref="H29:H32"/>
-    <mergeCell ref="A50:E50"/>
-    <mergeCell ref="I4:K6"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="H21:L21"/>
-    <mergeCell ref="H11:L11"/>
-    <mergeCell ref="H12:H14"/>
-    <mergeCell ref="H16:L16"/>
-    <mergeCell ref="H17:H19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>